<commit_message>
fix(bulk-import structures): clean feature and delete parent relations
</commit_message>
<xml_diff>
--- a/public/models/BulkImportStructures.xlsx
+++ b/public/models/BulkImportStructures.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">Nom usuel en français</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t xml:space="preserve">Date de fermeture approximative {O = Oui, N = Non}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent {rechercher le code}</t>
   </si>
 </sst>
 </file>
@@ -144,7 +141,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -165,12 +162,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -228,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,7 +232,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -250,10 +241,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,8 +327,8 @@
   </sheetPr>
   <dimension ref="A1:AL97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL7" activeCellId="0" sqref="AL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,25 +340,25 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -386,58 +373,58 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="AE1" s="3" t="s">
@@ -446,24 +433,22 @@
       <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="0" t="s">
-        <v>37</v>
-      </c>
+      <c r="AL1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
@@ -500,8 +485,8 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="6"/>
-      <c r="AG6" s="7"/>
+      <c r="K6" s="1"/>
+      <c r="AG6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
@@ -509,7 +494,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="M7" s="5"/>
-      <c r="AG7" s="7"/>
+      <c r="AG7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
fix(bulk-import): add new id for structures
</commit_message>
<xml_diff>
--- a/public/models/BulkImportStructures.xlsx
+++ b/public/models/BulkImportStructures.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">Nom usuel en français</t>
   </si>
@@ -74,6 +74,33 @@
   </si>
   <si>
     <t xml:space="preserve">Numéro siret [12345678901234]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant bibliothèque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant Crunchbase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant Dealroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant Google Scholar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant Rinngold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant idHal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant Grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant Crossref Funder Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant Finess Id</t>
   </si>
   <si>
     <t xml:space="preserve">Numéro RNSR [123456789X]</t>
@@ -229,7 +256,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,7 +273,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -335,22 +366,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL1048576"/>
+  <dimension ref="A1:AU86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="X1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="X5" activeCellId="0" sqref="X5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="40.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="40.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="40.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="59.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="56.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="18" style="2" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="59.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="56.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,31 +439,31 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
@@ -444,10 +475,10 @@
       <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
@@ -465,478 +496,494 @@
       <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="M2" s="6"/>
-      <c r="AG2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M2" s="7"/>
+      <c r="AP2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AJ3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP3" s="1"/>
+      <c r="AS3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="M4" s="6"/>
-      <c r="AG4" s="1"/>
-      <c r="AJ4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M4" s="7"/>
+      <c r="AP4" s="1"/>
+      <c r="AS4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="AG5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="M6" s="6"/>
-      <c r="AJ6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="7"/>
+      <c r="AS6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="AG7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="M8" s="6"/>
-      <c r="AG8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" s="7"/>
+      <c r="AP8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="AG9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="M10" s="6"/>
-      <c r="AG10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M10" s="7"/>
+      <c r="AP10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="AG11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="C12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="M12" s="6"/>
-      <c r="AG12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="7"/>
+      <c r="AP12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="AG13" s="1"/>
-      <c r="AJ13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP13" s="1"/>
+      <c r="AS13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="M14" s="6"/>
-      <c r="AG14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="7"/>
+      <c r="AP14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="AG15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="M16" s="6"/>
-      <c r="AG16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="7"/>
+      <c r="AP16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="AG17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="M18" s="6"/>
-      <c r="Y18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AG18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="7"/>
+      <c r="AH18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AP18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="AG19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="M20" s="6"/>
-      <c r="AG20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="7"/>
+      <c r="AP20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AG21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AJ21" s="1"/>
+      <c r="AP21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="M22" s="6"/>
-      <c r="AG22" s="1"/>
-      <c r="AJ22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M22" s="7"/>
+      <c r="AP22" s="1"/>
+      <c r="AS22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="AG23" s="1"/>
-      <c r="AJ23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP23" s="1"/>
+      <c r="AS23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="M24" s="6"/>
-      <c r="AA24" s="1"/>
-      <c r="AG24" s="1"/>
+      <c r="M24" s="7"/>
       <c r="AJ24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP24" s="1"/>
+      <c r="AS24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="AG25" s="1"/>
-      <c r="AJ25" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP25" s="1"/>
+      <c r="AS25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-      <c r="M26" s="6"/>
-      <c r="AG26" s="1"/>
-      <c r="AJ26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M26" s="7"/>
+      <c r="AP26" s="1"/>
+      <c r="AS26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AG27" s="1"/>
       <c r="AJ27" s="1"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP27" s="1"/>
+      <c r="AS27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="M28" s="6"/>
-      <c r="AG28" s="1"/>
-      <c r="AJ28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M28" s="7"/>
+      <c r="AP28" s="1"/>
+      <c r="AS28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="AG29" s="1"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="M30" s="6"/>
-      <c r="AG30" s="1"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M30" s="7"/>
+      <c r="AP30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="AG31" s="1"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="M32" s="6"/>
-      <c r="AG32" s="1"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M32" s="7"/>
+      <c r="AP32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="AG33" s="1"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="M34" s="6"/>
-      <c r="AG34" s="1"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M34" s="7"/>
+      <c r="AP34" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="AG35" s="1"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP35" s="1"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="M36" s="6"/>
-      <c r="Y36" s="1"/>
-      <c r="AG36" s="1"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M36" s="7"/>
+      <c r="AH36" s="1"/>
+      <c r="AP36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="AG37" s="1"/>
-      <c r="AJ37" s="1"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP37" s="1"/>
+      <c r="AS37" s="1"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="M38" s="6"/>
-      <c r="AG38" s="1"/>
-      <c r="AJ38" s="1"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M38" s="7"/>
+      <c r="AP38" s="1"/>
+      <c r="AS38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="AG39" s="1"/>
-      <c r="AJ39" s="1"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP39" s="1"/>
+      <c r="AS39" s="1"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="M40" s="6"/>
-      <c r="AG40" s="1"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M40" s="7"/>
+      <c r="AP40" s="1"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-      <c r="AG41" s="1"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP41" s="1"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="M42" s="6"/>
-      <c r="AG42" s="1"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M42" s="7"/>
+      <c r="AP42" s="1"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="AG43" s="1"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP43" s="1"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="M44" s="6"/>
-      <c r="AG44" s="1"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M44" s="7"/>
+      <c r="AP44" s="1"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
-      <c r="AG45" s="1"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP45" s="1"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="M46" s="6"/>
-      <c r="AG46" s="1"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M46" s="7"/>
+      <c r="AP46" s="1"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-      <c r="AG47" s="1"/>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP47" s="1"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="M48" s="6"/>
-      <c r="AG48" s="1"/>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M48" s="7"/>
+      <c r="AP48" s="1"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="AA49" s="1"/>
-      <c r="AG49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AJ49" s="1"/>
+      <c r="AP49" s="1"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
-      <c r="M50" s="6"/>
-      <c r="AG50" s="1"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M50" s="7"/>
+      <c r="AP50" s="1"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
-      <c r="AG51" s="1"/>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP51" s="1"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="M52" s="6"/>
-      <c r="AG52" s="1"/>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M52" s="7"/>
+      <c r="AP52" s="1"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="AG53" s="1"/>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP53" s="1"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="M54" s="6"/>
-      <c r="AG54" s="1"/>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M54" s="7"/>
+      <c r="AP54" s="1"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J55" s="1"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J56" s="1"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J57" s="1"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J58" s="1"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J59" s="1"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J60" s="1"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J61" s="1"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J62" s="1"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J63" s="1"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J64" s="1"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J65" s="1"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J66" s="1"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J67" s="1"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J68" s="1"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J69" s="1"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J70" s="1"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J71" s="1"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J72" s="1"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J73" s="1"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J74" s="1"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J75" s="1"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J76" s="1"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J77" s="1"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J78" s="1"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J79" s="1"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J80" s="1"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J81" s="1"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J82" s="1"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J83" s="1"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J84" s="1"/>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J85" s="1"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J86" s="1"/>
     </row>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>